<commit_message>
feat: now you may get unique fake values
</commit_message>
<xml_diff>
--- a/put candidate - RPA.xlsx
+++ b/put candidate - RPA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\lucas_hcx\desktop\repositories\eib-faker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694C8052-2438-45FE-9E18-4C4F4EE64BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FAFFA1-224D-441C-83D4-17E42EFC3CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1741,13 +1741,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="38" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1762,6 +1755,13 @@
     <xf numFmtId="0" fontId="21" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2121,8 +2121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:LS16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="CA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="CX6" sqref="CX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,475 +2623,475 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="21" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="21" t="s">
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="23"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="33"/>
       <c r="X2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="21" t="s">
+      <c r="Y2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="24" t="s">
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="26"/>
-      <c r="AO2" s="21" t="s">
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="30"/>
+      <c r="AO2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="AP2" s="22"/>
-      <c r="AQ2" s="22"/>
-      <c r="AR2" s="22"/>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="23"/>
-      <c r="AU2" s="24" t="s">
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="32"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="AV2" s="25"/>
-      <c r="AW2" s="25"/>
-      <c r="AX2" s="25"/>
-      <c r="AY2" s="25"/>
-      <c r="AZ2" s="25"/>
-      <c r="BA2" s="25"/>
-      <c r="BB2" s="25"/>
-      <c r="BC2" s="25"/>
-      <c r="BD2" s="25"/>
-      <c r="BE2" s="25"/>
-      <c r="BF2" s="25"/>
-      <c r="BG2" s="25"/>
-      <c r="BH2" s="25"/>
-      <c r="BI2" s="25"/>
-      <c r="BJ2" s="25"/>
-      <c r="BK2" s="25"/>
-      <c r="BL2" s="25"/>
-      <c r="BM2" s="25"/>
-      <c r="BN2" s="25"/>
-      <c r="BO2" s="25"/>
-      <c r="BP2" s="25"/>
-      <c r="BQ2" s="25"/>
-      <c r="BR2" s="25"/>
-      <c r="BS2" s="25"/>
-      <c r="BT2" s="26"/>
-      <c r="BU2" s="21" t="s">
+      <c r="AV2" s="29"/>
+      <c r="AW2" s="29"/>
+      <c r="AX2" s="29"/>
+      <c r="AY2" s="29"/>
+      <c r="AZ2" s="29"/>
+      <c r="BA2" s="29"/>
+      <c r="BB2" s="29"/>
+      <c r="BC2" s="29"/>
+      <c r="BD2" s="29"/>
+      <c r="BE2" s="29"/>
+      <c r="BF2" s="29"/>
+      <c r="BG2" s="29"/>
+      <c r="BH2" s="29"/>
+      <c r="BI2" s="29"/>
+      <c r="BJ2" s="29"/>
+      <c r="BK2" s="29"/>
+      <c r="BL2" s="29"/>
+      <c r="BM2" s="29"/>
+      <c r="BN2" s="29"/>
+      <c r="BO2" s="29"/>
+      <c r="BP2" s="29"/>
+      <c r="BQ2" s="29"/>
+      <c r="BR2" s="29"/>
+      <c r="BS2" s="29"/>
+      <c r="BT2" s="30"/>
+      <c r="BU2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="BV2" s="22"/>
-      <c r="BW2" s="22"/>
-      <c r="BX2" s="23"/>
-      <c r="BY2" s="24" t="s">
+      <c r="BV2" s="32"/>
+      <c r="BW2" s="32"/>
+      <c r="BX2" s="33"/>
+      <c r="BY2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="BZ2" s="26"/>
-      <c r="CA2" s="21" t="s">
+      <c r="BZ2" s="30"/>
+      <c r="CA2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="CB2" s="23"/>
-      <c r="CC2" s="24" t="s">
+      <c r="CB2" s="33"/>
+      <c r="CC2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="CD2" s="25"/>
-      <c r="CE2" s="25"/>
-      <c r="CF2" s="25"/>
-      <c r="CG2" s="25"/>
-      <c r="CH2" s="25"/>
-      <c r="CI2" s="25"/>
-      <c r="CJ2" s="25"/>
-      <c r="CK2" s="25"/>
-      <c r="CL2" s="25"/>
-      <c r="CM2" s="25"/>
-      <c r="CN2" s="26"/>
-      <c r="CO2" s="21" t="s">
+      <c r="CD2" s="29"/>
+      <c r="CE2" s="29"/>
+      <c r="CF2" s="29"/>
+      <c r="CG2" s="29"/>
+      <c r="CH2" s="29"/>
+      <c r="CI2" s="29"/>
+      <c r="CJ2" s="29"/>
+      <c r="CK2" s="29"/>
+      <c r="CL2" s="29"/>
+      <c r="CM2" s="29"/>
+      <c r="CN2" s="30"/>
+      <c r="CO2" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="CP2" s="22"/>
-      <c r="CQ2" s="22"/>
-      <c r="CR2" s="22"/>
-      <c r="CS2" s="22"/>
-      <c r="CT2" s="23"/>
-      <c r="CU2" s="24" t="s">
+      <c r="CP2" s="32"/>
+      <c r="CQ2" s="32"/>
+      <c r="CR2" s="32"/>
+      <c r="CS2" s="32"/>
+      <c r="CT2" s="33"/>
+      <c r="CU2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="CV2" s="25"/>
-      <c r="CW2" s="25"/>
-      <c r="CX2" s="25"/>
-      <c r="CY2" s="25"/>
-      <c r="CZ2" s="25"/>
-      <c r="DA2" s="25"/>
-      <c r="DB2" s="25"/>
-      <c r="DC2" s="25"/>
-      <c r="DD2" s="25"/>
-      <c r="DE2" s="25"/>
-      <c r="DF2" s="25"/>
-      <c r="DG2" s="25"/>
-      <c r="DH2" s="25"/>
-      <c r="DI2" s="25"/>
-      <c r="DJ2" s="25"/>
-      <c r="DK2" s="25"/>
-      <c r="DL2" s="25"/>
-      <c r="DM2" s="25"/>
-      <c r="DN2" s="26"/>
-      <c r="DO2" s="21" t="s">
+      <c r="CV2" s="29"/>
+      <c r="CW2" s="29"/>
+      <c r="CX2" s="29"/>
+      <c r="CY2" s="29"/>
+      <c r="CZ2" s="29"/>
+      <c r="DA2" s="29"/>
+      <c r="DB2" s="29"/>
+      <c r="DC2" s="29"/>
+      <c r="DD2" s="29"/>
+      <c r="DE2" s="29"/>
+      <c r="DF2" s="29"/>
+      <c r="DG2" s="29"/>
+      <c r="DH2" s="29"/>
+      <c r="DI2" s="29"/>
+      <c r="DJ2" s="29"/>
+      <c r="DK2" s="29"/>
+      <c r="DL2" s="29"/>
+      <c r="DM2" s="29"/>
+      <c r="DN2" s="30"/>
+      <c r="DO2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="DP2" s="22"/>
-      <c r="DQ2" s="22"/>
-      <c r="DR2" s="23"/>
-      <c r="DS2" s="24" t="s">
+      <c r="DP2" s="32"/>
+      <c r="DQ2" s="32"/>
+      <c r="DR2" s="33"/>
+      <c r="DS2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="DT2" s="26"/>
-      <c r="DU2" s="21" t="s">
+      <c r="DT2" s="30"/>
+      <c r="DU2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="DV2" s="22"/>
-      <c r="DW2" s="22"/>
-      <c r="DX2" s="22"/>
-      <c r="DY2" s="22"/>
-      <c r="DZ2" s="23"/>
-      <c r="EA2" s="24" t="s">
+      <c r="DV2" s="32"/>
+      <c r="DW2" s="32"/>
+      <c r="DX2" s="32"/>
+      <c r="DY2" s="32"/>
+      <c r="DZ2" s="33"/>
+      <c r="EA2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="EB2" s="25"/>
-      <c r="EC2" s="25"/>
-      <c r="ED2" s="25"/>
-      <c r="EE2" s="25"/>
-      <c r="EF2" s="26"/>
+      <c r="EB2" s="29"/>
+      <c r="EC2" s="29"/>
+      <c r="ED2" s="29"/>
+      <c r="EE2" s="29"/>
+      <c r="EF2" s="30"/>
       <c r="EG2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="EH2" s="24" t="s">
+      <c r="EH2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="EI2" s="25"/>
-      <c r="EJ2" s="26"/>
-      <c r="EK2" s="21" t="s">
+      <c r="EI2" s="29"/>
+      <c r="EJ2" s="30"/>
+      <c r="EK2" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="EL2" s="22"/>
-      <c r="EM2" s="22"/>
-      <c r="EN2" s="22"/>
-      <c r="EO2" s="22"/>
-      <c r="EP2" s="22"/>
-      <c r="EQ2" s="22"/>
-      <c r="ER2" s="22"/>
-      <c r="ES2" s="22"/>
-      <c r="ET2" s="22"/>
-      <c r="EU2" s="23"/>
-      <c r="EV2" s="24" t="s">
+      <c r="EL2" s="32"/>
+      <c r="EM2" s="32"/>
+      <c r="EN2" s="32"/>
+      <c r="EO2" s="32"/>
+      <c r="EP2" s="32"/>
+      <c r="EQ2" s="32"/>
+      <c r="ER2" s="32"/>
+      <c r="ES2" s="32"/>
+      <c r="ET2" s="32"/>
+      <c r="EU2" s="33"/>
+      <c r="EV2" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="EW2" s="25"/>
-      <c r="EX2" s="25"/>
-      <c r="EY2" s="25"/>
-      <c r="EZ2" s="25"/>
-      <c r="FA2" s="25"/>
-      <c r="FB2" s="25"/>
-      <c r="FC2" s="26"/>
-      <c r="FD2" s="21" t="s">
+      <c r="EW2" s="29"/>
+      <c r="EX2" s="29"/>
+      <c r="EY2" s="29"/>
+      <c r="EZ2" s="29"/>
+      <c r="FA2" s="29"/>
+      <c r="FB2" s="29"/>
+      <c r="FC2" s="30"/>
+      <c r="FD2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="FE2" s="23"/>
-      <c r="FF2" s="24" t="s">
+      <c r="FE2" s="33"/>
+      <c r="FF2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="FG2" s="25"/>
-      <c r="FH2" s="25"/>
-      <c r="FI2" s="25"/>
-      <c r="FJ2" s="25"/>
-      <c r="FK2" s="25"/>
-      <c r="FL2" s="25"/>
-      <c r="FM2" s="25"/>
-      <c r="FN2" s="25"/>
-      <c r="FO2" s="26"/>
-      <c r="FP2" s="21" t="s">
+      <c r="FG2" s="29"/>
+      <c r="FH2" s="29"/>
+      <c r="FI2" s="29"/>
+      <c r="FJ2" s="29"/>
+      <c r="FK2" s="29"/>
+      <c r="FL2" s="29"/>
+      <c r="FM2" s="29"/>
+      <c r="FN2" s="29"/>
+      <c r="FO2" s="30"/>
+      <c r="FP2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="FQ2" s="22"/>
-      <c r="FR2" s="22"/>
-      <c r="FS2" s="22"/>
-      <c r="FT2" s="23"/>
-      <c r="FU2" s="24" t="s">
+      <c r="FQ2" s="32"/>
+      <c r="FR2" s="32"/>
+      <c r="FS2" s="32"/>
+      <c r="FT2" s="33"/>
+      <c r="FU2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="FV2" s="25"/>
-      <c r="FW2" s="25"/>
-      <c r="FX2" s="25"/>
-      <c r="FY2" s="25"/>
-      <c r="FZ2" s="26"/>
-      <c r="GA2" s="21" t="s">
+      <c r="FV2" s="29"/>
+      <c r="FW2" s="29"/>
+      <c r="FX2" s="29"/>
+      <c r="FY2" s="29"/>
+      <c r="FZ2" s="30"/>
+      <c r="GA2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="GB2" s="23"/>
-      <c r="GC2" s="24" t="s">
+      <c r="GB2" s="33"/>
+      <c r="GC2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="GD2" s="26"/>
+      <c r="GD2" s="30"/>
       <c r="GE2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="GF2" s="24" t="s">
+      <c r="GF2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="GG2" s="25"/>
-      <c r="GH2" s="26"/>
+      <c r="GG2" s="29"/>
+      <c r="GH2" s="30"/>
       <c r="GI2" s="4" t="s">
         <v>33</v>
       </c>
       <c r="GJ2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="GK2" s="21" t="s">
+      <c r="GK2" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="GL2" s="23"/>
-      <c r="GM2" s="24" t="s">
+      <c r="GL2" s="33"/>
+      <c r="GM2" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="GN2" s="25"/>
-      <c r="GO2" s="26"/>
-      <c r="GP2" s="21" t="s">
+      <c r="GN2" s="29"/>
+      <c r="GO2" s="30"/>
+      <c r="GP2" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="GQ2" s="22"/>
-      <c r="GR2" s="23"/>
+      <c r="GQ2" s="32"/>
+      <c r="GR2" s="33"/>
       <c r="GS2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="GT2" s="21" t="s">
+      <c r="GT2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="GU2" s="22"/>
-      <c r="GV2" s="22"/>
-      <c r="GW2" s="22"/>
-      <c r="GX2" s="23"/>
-      <c r="GY2" s="24" t="s">
+      <c r="GU2" s="32"/>
+      <c r="GV2" s="32"/>
+      <c r="GW2" s="32"/>
+      <c r="GX2" s="33"/>
+      <c r="GY2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="GZ2" s="25"/>
-      <c r="HA2" s="25"/>
-      <c r="HB2" s="25"/>
-      <c r="HC2" s="25"/>
-      <c r="HD2" s="25"/>
-      <c r="HE2" s="25"/>
-      <c r="HF2" s="25"/>
-      <c r="HG2" s="26"/>
-      <c r="HH2" s="21" t="s">
+      <c r="GZ2" s="29"/>
+      <c r="HA2" s="29"/>
+      <c r="HB2" s="29"/>
+      <c r="HC2" s="29"/>
+      <c r="HD2" s="29"/>
+      <c r="HE2" s="29"/>
+      <c r="HF2" s="29"/>
+      <c r="HG2" s="30"/>
+      <c r="HH2" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="HI2" s="22"/>
-      <c r="HJ2" s="22"/>
-      <c r="HK2" s="22"/>
-      <c r="HL2" s="22"/>
-      <c r="HM2" s="23"/>
+      <c r="HI2" s="32"/>
+      <c r="HJ2" s="32"/>
+      <c r="HK2" s="32"/>
+      <c r="HL2" s="32"/>
+      <c r="HM2" s="33"/>
       <c r="HN2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="HO2" s="21" t="s">
+      <c r="HO2" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="HP2" s="22"/>
-      <c r="HQ2" s="23"/>
-      <c r="HR2" s="24" t="s">
+      <c r="HP2" s="32"/>
+      <c r="HQ2" s="33"/>
+      <c r="HR2" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="HS2" s="25"/>
-      <c r="HT2" s="25"/>
-      <c r="HU2" s="25"/>
-      <c r="HV2" s="25"/>
-      <c r="HW2" s="25"/>
-      <c r="HX2" s="25"/>
-      <c r="HY2" s="25"/>
-      <c r="HZ2" s="25"/>
-      <c r="IA2" s="25"/>
-      <c r="IB2" s="26"/>
-      <c r="IC2" s="21" t="s">
+      <c r="HS2" s="29"/>
+      <c r="HT2" s="29"/>
+      <c r="HU2" s="29"/>
+      <c r="HV2" s="29"/>
+      <c r="HW2" s="29"/>
+      <c r="HX2" s="29"/>
+      <c r="HY2" s="29"/>
+      <c r="HZ2" s="29"/>
+      <c r="IA2" s="29"/>
+      <c r="IB2" s="30"/>
+      <c r="IC2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="ID2" s="22"/>
-      <c r="IE2" s="22"/>
-      <c r="IF2" s="22"/>
-      <c r="IG2" s="22"/>
-      <c r="IH2" s="22"/>
-      <c r="II2" s="22"/>
-      <c r="IJ2" s="23"/>
-      <c r="IK2" s="24" t="s">
+      <c r="ID2" s="32"/>
+      <c r="IE2" s="32"/>
+      <c r="IF2" s="32"/>
+      <c r="IG2" s="32"/>
+      <c r="IH2" s="32"/>
+      <c r="II2" s="32"/>
+      <c r="IJ2" s="33"/>
+      <c r="IK2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="IL2" s="26"/>
-      <c r="IM2" s="21" t="s">
+      <c r="IL2" s="30"/>
+      <c r="IM2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="IN2" s="22"/>
-      <c r="IO2" s="22"/>
-      <c r="IP2" s="22"/>
-      <c r="IQ2" s="22"/>
-      <c r="IR2" s="22"/>
-      <c r="IS2" s="22"/>
-      <c r="IT2" s="22"/>
-      <c r="IU2" s="22"/>
-      <c r="IV2" s="23"/>
-      <c r="IW2" s="24" t="s">
+      <c r="IN2" s="32"/>
+      <c r="IO2" s="32"/>
+      <c r="IP2" s="32"/>
+      <c r="IQ2" s="32"/>
+      <c r="IR2" s="32"/>
+      <c r="IS2" s="32"/>
+      <c r="IT2" s="32"/>
+      <c r="IU2" s="32"/>
+      <c r="IV2" s="33"/>
+      <c r="IW2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="IX2" s="25"/>
-      <c r="IY2" s="25"/>
-      <c r="IZ2" s="25"/>
-      <c r="JA2" s="26"/>
-      <c r="JB2" s="21" t="s">
+      <c r="IX2" s="29"/>
+      <c r="IY2" s="29"/>
+      <c r="IZ2" s="29"/>
+      <c r="JA2" s="30"/>
+      <c r="JB2" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="JC2" s="22"/>
-      <c r="JD2" s="22"/>
-      <c r="JE2" s="22"/>
-      <c r="JF2" s="22"/>
-      <c r="JG2" s="23"/>
-      <c r="JH2" s="24" t="s">
+      <c r="JC2" s="32"/>
+      <c r="JD2" s="32"/>
+      <c r="JE2" s="32"/>
+      <c r="JF2" s="32"/>
+      <c r="JG2" s="33"/>
+      <c r="JH2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="JI2" s="26"/>
-      <c r="JJ2" s="21" t="s">
+      <c r="JI2" s="30"/>
+      <c r="JJ2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="JK2" s="23"/>
+      <c r="JK2" s="33"/>
       <c r="JL2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="JM2" s="21" t="s">
+      <c r="JM2" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="JN2" s="22"/>
-      <c r="JO2" s="23"/>
+      <c r="JN2" s="32"/>
+      <c r="JO2" s="33"/>
       <c r="JP2" s="3" t="s">
         <v>53</v>
       </c>
       <c r="JQ2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="JR2" s="24" t="s">
+      <c r="JR2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="JS2" s="26"/>
-      <c r="JT2" s="21" t="s">
+      <c r="JS2" s="30"/>
+      <c r="JT2" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="JU2" s="22"/>
-      <c r="JV2" s="23"/>
-      <c r="JW2" s="24" t="s">
+      <c r="JU2" s="32"/>
+      <c r="JV2" s="33"/>
+      <c r="JW2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="JX2" s="25"/>
-      <c r="JY2" s="26"/>
+      <c r="JX2" s="29"/>
+      <c r="JY2" s="30"/>
       <c r="JZ2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="KA2" s="24" t="s">
+      <c r="KA2" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="KB2" s="25"/>
-      <c r="KC2" s="25"/>
-      <c r="KD2" s="25"/>
-      <c r="KE2" s="26"/>
-      <c r="KF2" s="21" t="s">
+      <c r="KB2" s="29"/>
+      <c r="KC2" s="29"/>
+      <c r="KD2" s="29"/>
+      <c r="KE2" s="30"/>
+      <c r="KF2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="KG2" s="22"/>
-      <c r="KH2" s="23"/>
-      <c r="KI2" s="24" t="s">
+      <c r="KG2" s="32"/>
+      <c r="KH2" s="33"/>
+      <c r="KI2" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="KJ2" s="25"/>
-      <c r="KK2" s="26"/>
-      <c r="KL2" s="21" t="s">
+      <c r="KJ2" s="29"/>
+      <c r="KK2" s="30"/>
+      <c r="KL2" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="KM2" s="22"/>
-      <c r="KN2" s="22"/>
-      <c r="KO2" s="22"/>
-      <c r="KP2" s="22"/>
-      <c r="KQ2" s="22"/>
-      <c r="KR2" s="22"/>
-      <c r="KS2" s="22"/>
-      <c r="KT2" s="23"/>
+      <c r="KM2" s="32"/>
+      <c r="KN2" s="32"/>
+      <c r="KO2" s="32"/>
+      <c r="KP2" s="32"/>
+      <c r="KQ2" s="32"/>
+      <c r="KR2" s="32"/>
+      <c r="KS2" s="32"/>
+      <c r="KT2" s="33"/>
       <c r="KU2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="KV2" s="21" t="s">
+      <c r="KV2" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="KW2" s="22"/>
-      <c r="KX2" s="23"/>
-      <c r="KY2" s="24" t="s">
+      <c r="KW2" s="32"/>
+      <c r="KX2" s="33"/>
+      <c r="KY2" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="KZ2" s="25"/>
-      <c r="LA2" s="25"/>
-      <c r="LB2" s="25"/>
-      <c r="LC2" s="25"/>
-      <c r="LD2" s="25"/>
-      <c r="LE2" s="26"/>
+      <c r="KZ2" s="29"/>
+      <c r="LA2" s="29"/>
+      <c r="LB2" s="29"/>
+      <c r="LC2" s="29"/>
+      <c r="LD2" s="29"/>
+      <c r="LE2" s="30"/>
       <c r="LF2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="LG2" s="24" t="s">
+      <c r="LG2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="LH2" s="26"/>
-      <c r="LI2" s="21" t="s">
+      <c r="LH2" s="30"/>
+      <c r="LI2" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="LJ2" s="22"/>
-      <c r="LK2" s="23"/>
-      <c r="LL2" s="24" t="s">
+      <c r="LJ2" s="32"/>
+      <c r="LK2" s="33"/>
+      <c r="LL2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="LM2" s="26"/>
-      <c r="LN2" s="21" t="s">
+      <c r="LM2" s="30"/>
+      <c r="LN2" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="LO2" s="22"/>
-      <c r="LP2" s="22"/>
-      <c r="LQ2" s="22"/>
-      <c r="LR2" s="23"/>
+      <c r="LO2" s="32"/>
+      <c r="LP2" s="32"/>
+      <c r="LQ2" s="32"/>
+      <c r="LR2" s="33"/>
       <c r="LS2" s="3" t="s">
         <v>65</v>
       </c>
@@ -6086,7 +6086,7 @@
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="21" t="s">
         <v>323</v>
       </c>
       <c r="K6" s="11" t="s">
@@ -6095,10 +6095,10 @@
       <c r="N6" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="AO6" s="29" t="s">
+      <c r="AO6" s="22" t="s">
         <v>324</v>
       </c>
-      <c r="AP6" s="29" t="s">
+      <c r="AP6" s="22" t="s">
         <v>331</v>
       </c>
       <c r="AQ6" s="17">
@@ -6107,7 +6107,7 @@
       <c r="AS6" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="AU6" s="29" t="s">
+      <c r="AU6" s="22" t="s">
         <v>325</v>
       </c>
       <c r="AV6" s="11" t="s">
@@ -6128,20 +6128,20 @@
       <c r="BT6" s="11">
         <v>4841195</v>
       </c>
-      <c r="BY6" s="30" t="s">
+      <c r="BY6" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="BZ6" s="30" t="s">
+      <c r="BZ6" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="CA6" s="30">
+      <c r="CA6" s="23">
         <v>1</v>
       </c>
-      <c r="CC6" s="30">
+      <c r="CC6" s="23">
         <v>1</v>
       </c>
       <c r="CE6" s="18"/>
-      <c r="CG6" s="31" t="s">
+      <c r="CG6" s="24" t="s">
         <v>326</v>
       </c>
       <c r="CU6" s="11" t="s">
@@ -6150,28 +6150,28 @@
       <c r="CV6" s="14">
         <v>34503</v>
       </c>
-      <c r="CW6" s="32" t="s">
+      <c r="CW6" s="25" t="s">
         <v>325</v>
       </c>
-      <c r="CX6" s="30" t="s">
+      <c r="CX6" s="15" t="s">
         <v>332</v>
       </c>
       <c r="CY6" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="DE6" s="32" t="s">
+      <c r="DE6" s="25" t="s">
         <v>327</v>
       </c>
-      <c r="DH6" s="32" t="s">
+      <c r="DH6" s="25" t="s">
         <v>325</v>
       </c>
-      <c r="GJ6" s="33" t="s">
+      <c r="GJ6" s="26" t="s">
         <v>328</v>
       </c>
-      <c r="GK6" s="30">
+      <c r="GK6" s="23">
         <v>1</v>
       </c>
-      <c r="GL6" s="32" t="s">
+      <c r="GL6" s="25" t="s">
         <v>329</v>
       </c>
       <c r="GM6" s="6"/>
@@ -6274,16 +6274,16 @@
       <c r="KF6" s="7"/>
       <c r="KG6" s="6"/>
       <c r="KH6" s="6"/>
-      <c r="KI6" s="30">
+      <c r="KI6" s="23">
         <v>1</v>
       </c>
       <c r="KL6" s="12">
         <v>60082064016</v>
       </c>
-      <c r="KM6" s="32" t="s">
+      <c r="KM6" s="25" t="s">
         <v>330</v>
       </c>
-      <c r="KN6" s="32" t="s">
+      <c r="KN6" s="25" t="s">
         <v>325</v>
       </c>
     </row>
@@ -8429,6 +8429,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="LN2:LR2"/>
+    <mergeCell ref="JT2:JV2"/>
+    <mergeCell ref="JW2:JY2"/>
+    <mergeCell ref="KA2:KE2"/>
+    <mergeCell ref="KF2:KH2"/>
+    <mergeCell ref="KI2:KK2"/>
+    <mergeCell ref="KL2:KT2"/>
+    <mergeCell ref="KV2:KX2"/>
+    <mergeCell ref="KY2:LE2"/>
+    <mergeCell ref="LG2:LH2"/>
+    <mergeCell ref="LI2:LK2"/>
+    <mergeCell ref="LL2:LM2"/>
+    <mergeCell ref="JR2:JS2"/>
+    <mergeCell ref="HH2:HM2"/>
+    <mergeCell ref="HO2:HQ2"/>
+    <mergeCell ref="HR2:IB2"/>
+    <mergeCell ref="IC2:IJ2"/>
+    <mergeCell ref="IK2:IL2"/>
+    <mergeCell ref="IM2:IV2"/>
+    <mergeCell ref="IW2:JA2"/>
+    <mergeCell ref="JB2:JG2"/>
+    <mergeCell ref="JH2:JI2"/>
+    <mergeCell ref="JJ2:JK2"/>
+    <mergeCell ref="JM2:JO2"/>
+    <mergeCell ref="EK2:EU2"/>
+    <mergeCell ref="GY2:HG2"/>
+    <mergeCell ref="FD2:FE2"/>
+    <mergeCell ref="FF2:FO2"/>
+    <mergeCell ref="FP2:FT2"/>
+    <mergeCell ref="FU2:FZ2"/>
+    <mergeCell ref="GA2:GB2"/>
+    <mergeCell ref="GC2:GD2"/>
+    <mergeCell ref="GF2:GH2"/>
+    <mergeCell ref="GK2:GL2"/>
+    <mergeCell ref="GM2:GO2"/>
+    <mergeCell ref="GP2:GR2"/>
+    <mergeCell ref="GT2:GX2"/>
+    <mergeCell ref="DO2:DR2"/>
+    <mergeCell ref="DS2:DT2"/>
+    <mergeCell ref="DU2:DZ2"/>
+    <mergeCell ref="EA2:EF2"/>
+    <mergeCell ref="EH2:EJ2"/>
     <mergeCell ref="A1:LS1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
@@ -8445,48 +8487,6 @@
     <mergeCell ref="CC2:CN2"/>
     <mergeCell ref="CO2:CT2"/>
     <mergeCell ref="CU2:DN2"/>
-    <mergeCell ref="DO2:DR2"/>
-    <mergeCell ref="DS2:DT2"/>
-    <mergeCell ref="DU2:DZ2"/>
-    <mergeCell ref="EA2:EF2"/>
-    <mergeCell ref="EH2:EJ2"/>
-    <mergeCell ref="EK2:EU2"/>
-    <mergeCell ref="GY2:HG2"/>
-    <mergeCell ref="FD2:FE2"/>
-    <mergeCell ref="FF2:FO2"/>
-    <mergeCell ref="FP2:FT2"/>
-    <mergeCell ref="FU2:FZ2"/>
-    <mergeCell ref="GA2:GB2"/>
-    <mergeCell ref="GC2:GD2"/>
-    <mergeCell ref="GF2:GH2"/>
-    <mergeCell ref="GK2:GL2"/>
-    <mergeCell ref="GM2:GO2"/>
-    <mergeCell ref="GP2:GR2"/>
-    <mergeCell ref="GT2:GX2"/>
-    <mergeCell ref="JR2:JS2"/>
-    <mergeCell ref="HH2:HM2"/>
-    <mergeCell ref="HO2:HQ2"/>
-    <mergeCell ref="HR2:IB2"/>
-    <mergeCell ref="IC2:IJ2"/>
-    <mergeCell ref="IK2:IL2"/>
-    <mergeCell ref="IM2:IV2"/>
-    <mergeCell ref="IW2:JA2"/>
-    <mergeCell ref="JB2:JG2"/>
-    <mergeCell ref="JH2:JI2"/>
-    <mergeCell ref="JJ2:JK2"/>
-    <mergeCell ref="JM2:JO2"/>
-    <mergeCell ref="LN2:LR2"/>
-    <mergeCell ref="JT2:JV2"/>
-    <mergeCell ref="JW2:JY2"/>
-    <mergeCell ref="KA2:KE2"/>
-    <mergeCell ref="KF2:KH2"/>
-    <mergeCell ref="KI2:KK2"/>
-    <mergeCell ref="KL2:KT2"/>
-    <mergeCell ref="KV2:KX2"/>
-    <mergeCell ref="KY2:LE2"/>
-    <mergeCell ref="LG2:LH2"/>
-    <mergeCell ref="LI2:LK2"/>
-    <mergeCell ref="LL2:LM2"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <dataValidations count="68">
@@ -8704,16 +8704,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="31013da8-747d-49b5-9af0-03e41a79c882" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fe4e2c59-8198-4aea-a184-9f9eaa6429f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8963,22 +8959,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="31013da8-747d-49b5-9af0-03e41a79c882" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fe4e2c59-8198-4aea-a184-9f9eaa6429f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E54A0EFC-B74F-4B3C-A99A-E3AD54BA0B9F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F08C7535-BA2E-4CF9-BEC5-BDE470A2D69E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="31013da8-747d-49b5-9af0-03e41a79c882"/>
-    <ds:schemaRef ds:uri="fe4e2c59-8198-4aea-a184-9f9eaa6429f5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9004,9 +9000,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F08C7535-BA2E-4CF9-BEC5-BDE470A2D69E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E54A0EFC-B74F-4B3C-A99A-E3AD54BA0B9F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="31013da8-747d-49b5-9af0-03e41a79c882"/>
+    <ds:schemaRef ds:uri="fe4e2c59-8198-4aea-a184-9f9eaa6429f5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>